<commit_message>
Docs/development: update NOP demo
</commit_message>
<xml_diff>
--- a/docs/100.development/800.nop/800.demo/files/nop-demo.orm.v0.xlsx
+++ b/docs/100.development/800.nop/800.demo/files/nop-demo.orm.v0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>#变量名</t>
   </si>
@@ -28,6 +28,9 @@
     <t>registerShortName</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>实体名为包含包名的全类名，如果 registerShortName 设置为 true，则也可以通过去除包名的短类名来访问实体</t>
   </si>
   <si>
@@ -43,7 +46,7 @@
     <t>entityPackageName</t>
   </si>
   <si>
-    <t>nop.demo.dao.entity</t>
+    <t>io.nop.demo.dao.entity</t>
   </si>
   <si>
     <t>实体对象所在的包名，一般应该是 xxx.dao.entity，例如 io.nop.sys.dao.entity</t>
@@ -52,7 +55,7 @@
     <t>basePackageName</t>
   </si>
   <si>
-    <t>nop.demo</t>
+    <t>io.nop.demo</t>
   </si>
   <si>
     <t>所有子模块的父包名, 例如 io.nop.sys</t>
@@ -61,9 +64,6 @@
     <t>maven.groupId</t>
   </si>
   <si>
-    <t>io.nop.demo</t>
-  </si>
-  <si>
     <t>主工程的 groupId</t>
   </si>
   <si>
@@ -88,7 +88,7 @@
     <t>2.0.0-SNAPSHOT</t>
   </si>
   <si>
-    <t>Nop 平台的版本号</t>
+    <t>NOP 平台的版本号</t>
   </si>
   <si>
     <t>dialect</t>
@@ -105,9 +105,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -125,6 +125,59 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -132,37 +185,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -170,16 +246,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,82 +268,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -284,13 +284,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,43 +392,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,43 +446,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,73 +464,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,41 +493,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -562,11 +532,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -574,8 +550,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,153 +566,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -753,7 +753,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1107,52 +1107,52 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="b">
-        <v>1</v>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="66" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="33" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>16</v>
@@ -1163,7 +1163,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>18</v>

</xml_diff>